<commit_message>
Renaming img_crop_labels & imgtoexcel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Menu Items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Linked Dish" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option Groups" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Linked Options" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Options" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Menu Items" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Linked Dish" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Option Groups" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Linked Options" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Options" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
edited copyto clipboard button and minor mods to make sheet part work
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Options" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Items" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Options" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Fixed changing sheet in excel_generator
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Options" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Options" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
generate excel button working
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Options" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Items" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Option Group" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Options" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,50 +465,189 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mala</t>
+          <t>Larger Plates</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mala</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
+          <t>Nichols Smoked Chicken Breast</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>3.5</v>
+        <v>36</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Soup or Dry,Spicy Level,Ingredient</t>
+          <t>Sides</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Grilled Fish</t>
+          <t>Larger Plates</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Grilled Fish</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
+          <t>Scottsdale Pork Belly</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>27.2</v>
+        <v>36</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Fish Flavour,Grilled Fish Addon</t>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Larger Plates</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Wild Clover Lamb</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>40</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Larger Plates</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rannoch Farm Quail</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>37</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Larger Plates</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pan Roasted Fish</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>37</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Larger Plates</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Braised Lentils</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>30</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Steak Plates</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>300g Porterhouse</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>36</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sides, Doneness</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Steak Plates</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>300g Scotch Fillet</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>42</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Steak Plates</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>220g Eye Fillet</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sides</t>
         </is>
       </c>
     </row>
@@ -551,27 +690,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Soup or Dry</t>
-        </is>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
+          <t>Doneness</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Spicy Level</t>
-        </is>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -585,7 +732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,12 +760,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Soup or Dry</t>
+          <t>Doneness</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dry</t>
+          <t>Medium Rare</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -628,31 +775,136 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Soup or Dry</t>
+          <t>Doneness</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Soup</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Spicy Level</t>
+          <t>Doneness</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Level 1 - Less Spicy</t>
+          <t>Well Done</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Doneness</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Overcooked</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Doneness</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Burnt</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>French Fries</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Garden Veggie</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Coleslaw</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Mashed Potato</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sides</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tasty Rice</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>